<commit_message>
All completed experiments - OS S4 lab
</commit_message>
<xml_diff>
--- a/ExperimentsDocs/Index.xlsx
+++ b/ExperimentsDocs/Index.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\repositories\S4-OSlab\ExperimentsDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9CA4C9-BACC-4AED-8AE9-27388A8BFC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FFCA09-5F77-4064-B728-B24B68F39A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>CONTENTS</t>
   </si>
@@ -70,6 +70,21 @@
   </si>
   <si>
     <t>Dining Philosophors Problem</t>
+  </si>
+  <si>
+    <t>Memory Allocation Methods</t>
+  </si>
+  <si>
+    <t>Page Replacement Algorithms</t>
+  </si>
+  <si>
+    <t>Deadlock Avoidance - Banker's Algorithm</t>
+  </si>
+  <si>
+    <t>Deadlock Detection Algorithm</t>
+  </si>
+  <si>
+    <t>Disk Scheduling algorithm</t>
   </si>
 </sst>
 </file>
@@ -475,7 +490,7 @@
   <dimension ref="A1:AMJ27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.8" x14ac:dyDescent="0.25"/>
@@ -618,33 +633,63 @@
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" ht="26.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="7">
+        <v>45420</v>
+      </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" ht="26.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="4"/>
+      <c r="A13" s="4">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="7">
+        <v>45421</v>
+      </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" ht="26.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="4"/>
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="7">
+        <v>45421</v>
+      </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" ht="26.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4"/>
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="7">
+        <v>45421</v>
+      </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" ht="26.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="4">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="7">
+        <v>45421</v>
+      </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" ht="26.85" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>